<commit_message>
change fasli to quarterly
</commit_message>
<xml_diff>
--- a/database/industries/folad/fakhouz/balancesheet/yearly.xlsx
+++ b/database/industries/folad/fakhouz/balancesheet/yearly.xlsx
@@ -192,6 +192,11 @@
     <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="10" max="10" width="29" customWidth="1"/>
+    <col min="11" max="11" width="29" customWidth="1"/>
+    <col min="12" max="12" width="29" customWidth="1"/>
+    <col min="13" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -216,6 +221,21 @@
       <c r="H1" s="2">
         <v/>
       </c>
+      <c r="I1" s="2">
+        <v/>
+      </c>
+      <c r="J1" s="2">
+        <v/>
+      </c>
+      <c r="K1" s="2">
+        <v/>
+      </c>
+      <c r="L1" s="2">
+        <v/>
+      </c>
+      <c r="M1" s="2">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="3" t="inlineStr">
@@ -241,6 +261,21 @@
       <c r="H2" s="2">
         <v/>
       </c>
+      <c r="I2" s="2">
+        <v/>
+      </c>
+      <c r="J2" s="2">
+        <v/>
+      </c>
+      <c r="K2" s="2">
+        <v/>
+      </c>
+      <c r="L2" s="2">
+        <v/>
+      </c>
+      <c r="M2" s="2">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="4" t="inlineStr">
@@ -266,6 +301,21 @@
       <c r="H3" s="2">
         <v/>
       </c>
+      <c r="I3" s="2">
+        <v/>
+      </c>
+      <c r="J3" s="2">
+        <v/>
+      </c>
+      <c r="K3" s="2">
+        <v/>
+      </c>
+      <c r="L3" s="2">
+        <v/>
+      </c>
+      <c r="M3" s="2">
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="2">
@@ -289,6 +339,21 @@
       <c r="H4" s="2">
         <v/>
       </c>
+      <c r="I4" s="2">
+        <v/>
+      </c>
+      <c r="J4" s="2">
+        <v/>
+      </c>
+      <c r="K4" s="2">
+        <v/>
+      </c>
+      <c r="L4" s="2">
+        <v/>
+      </c>
+      <c r="M4" s="2">
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="5" t="inlineStr">
@@ -314,6 +379,21 @@
       <c r="H5" s="5">
         <v/>
       </c>
+      <c r="I5" s="5">
+        <v/>
+      </c>
+      <c r="J5" s="5">
+        <v/>
+      </c>
+      <c r="K5" s="5">
+        <v/>
+      </c>
+      <c r="L5" s="5">
+        <v/>
+      </c>
+      <c r="M5" s="5">
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="6" t="inlineStr">
@@ -339,6 +419,21 @@
       <c r="H6" s="5">
         <v/>
       </c>
+      <c r="I6" s="5">
+        <v/>
+      </c>
+      <c r="J6" s="5">
+        <v/>
+      </c>
+      <c r="K6" s="5">
+        <v/>
+      </c>
+      <c r="L6" s="5">
+        <v/>
+      </c>
+      <c r="M6" s="5">
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="2">
@@ -362,6 +457,21 @@
       <c r="H7" s="2">
         <v/>
       </c>
+      <c r="I7" s="2">
+        <v/>
+      </c>
+      <c r="J7" s="2">
+        <v/>
+      </c>
+      <c r="K7" s="2">
+        <v/>
+      </c>
+      <c r="L7" s="2">
+        <v/>
+      </c>
+      <c r="M7" s="2">
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="8" t="inlineStr">
@@ -374,25 +484,50 @@
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
+          <t>12 ماهه منتهی به 1391/12</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1392/12</t>
+        </is>
+      </c>
+      <c r="F8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1393/12</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1394/12</t>
+        </is>
+      </c>
+      <c r="H8" s="7" t="inlineStr">
+        <is>
+          <t>12 ماهه منتهی به 1395/12</t>
+        </is>
+      </c>
+      <c r="I8" s="7" t="inlineStr">
+        <is>
           <t>12 ماهه منتهی به 1396/12</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr">
+      <c r="J8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1397/12</t>
         </is>
       </c>
-      <c r="F8" s="7" t="inlineStr">
+      <c r="K8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1398/12</t>
         </is>
       </c>
-      <c r="G8" s="7" t="inlineStr">
+      <c r="L8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1399/12</t>
         </is>
       </c>
-      <c r="H8" s="7" t="inlineStr">
+      <c r="M8" s="7" t="inlineStr">
         <is>
           <t>12 ماهه منتهی به 1400/12</t>
         </is>
@@ -409,27 +544,52 @@
       </c>
       <c r="D9" s="10" t="inlineStr">
         <is>
+          <t>1393-02-17 (7)</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="inlineStr">
+        <is>
+          <t>1394-03-09 (8)</t>
+        </is>
+      </c>
+      <c r="F9" s="10" t="inlineStr">
+        <is>
+          <t>1395-04-20 (8)</t>
+        </is>
+      </c>
+      <c r="G9" s="10" t="inlineStr">
+        <is>
+          <t>1396-03-30 (9)</t>
+        </is>
+      </c>
+      <c r="H9" s="10" t="inlineStr">
+        <is>
+          <t>1397-03-19 (10)</t>
+        </is>
+      </c>
+      <c r="I9" s="10" t="inlineStr">
+        <is>
           <t>1398-03-08 (8)</t>
         </is>
       </c>
-      <c r="E9" s="10" t="inlineStr">
+      <c r="J9" s="10" t="inlineStr">
         <is>
           <t>1399-05-01 (9)</t>
         </is>
       </c>
-      <c r="F9" s="10" t="inlineStr">
+      <c r="K9" s="10" t="inlineStr">
         <is>
           <t>1400-03-30 (9)</t>
         </is>
       </c>
-      <c r="G9" s="10" t="inlineStr">
+      <c r="L9" s="10" t="inlineStr">
         <is>
           <t>1401-04-16 (10)</t>
         </is>
       </c>
-      <c r="H9" s="10" t="inlineStr">
-        <is>
-          <t>1401-04-30 (3)</t>
+      <c r="M9" s="10" t="inlineStr">
+        <is>
+          <t>1401-07-30 (5)</t>
         </is>
       </c>
     </row>
@@ -455,6 +615,21 @@
       <c r="H10" s="12">
         <v/>
       </c>
+      <c r="I10" s="12">
+        <v/>
+      </c>
+      <c r="J10" s="12">
+        <v/>
+      </c>
+      <c r="K10" s="12">
+        <v/>
+      </c>
+      <c r="L10" s="12">
+        <v/>
+      </c>
+      <c r="M10" s="12">
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="13" t="inlineStr">
@@ -480,6 +655,21 @@
       <c r="H11" s="14">
         <v/>
       </c>
+      <c r="I11" s="14">
+        <v/>
+      </c>
+      <c r="J11" s="14">
+        <v/>
+      </c>
+      <c r="K11" s="14">
+        <v/>
+      </c>
+      <c r="L11" s="14">
+        <v/>
+      </c>
+      <c r="M11" s="14">
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="15" t="inlineStr">
@@ -491,18 +681,33 @@
         <v/>
       </c>
       <c r="D12" s="16">
+        <v>2957336</v>
+      </c>
+      <c r="E12" s="16">
+        <v>1746204</v>
+      </c>
+      <c r="F12" s="16">
+        <v>709847</v>
+      </c>
+      <c r="G12" s="16">
+        <v>795859</v>
+      </c>
+      <c r="H12" s="16">
+        <v>2693864</v>
+      </c>
+      <c r="I12" s="16">
         <v>2571498</v>
       </c>
-      <c r="E12" s="16">
+      <c r="J12" s="16">
         <v>4693944</v>
       </c>
-      <c r="F12" s="16">
+      <c r="K12" s="16">
         <v>7650719</v>
       </c>
-      <c r="G12" s="16">
+      <c r="L12" s="16">
         <v>31294267</v>
       </c>
-      <c r="H12" s="16">
+      <c r="M12" s="16">
         <v>11515059</v>
       </c>
     </row>
@@ -516,18 +721,33 @@
         <v/>
       </c>
       <c r="D13" s="12">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12">
+        <v>2976151</v>
+      </c>
+      <c r="F13" s="12">
+        <v>2000000</v>
+      </c>
+      <c r="G13" s="12">
         <v>1500000</v>
       </c>
-      <c r="E13" s="12">
+      <c r="H13" s="12">
         <v>1500000</v>
       </c>
-      <c r="F13" s="12">
+      <c r="I13" s="12">
+        <v>1500000</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1500000</v>
+      </c>
+      <c r="K13" s="12">
         <v>2690000</v>
       </c>
-      <c r="G13" s="12">
+      <c r="L13" s="12">
         <v>3657884</v>
       </c>
-      <c r="H13" s="12">
+      <c r="M13" s="12">
         <v>2690000</v>
       </c>
     </row>
@@ -541,19 +761,34 @@
         <v/>
       </c>
       <c r="D14" s="16">
+        <v>7361348</v>
+      </c>
+      <c r="E14" s="16">
+        <v>9038227</v>
+      </c>
+      <c r="F14" s="16">
+        <v>6932386</v>
+      </c>
+      <c r="G14" s="16">
+        <v>9456942</v>
+      </c>
+      <c r="H14" s="16">
+        <v>7334791</v>
+      </c>
+      <c r="I14" s="16">
         <v>10790608</v>
       </c>
-      <c r="E14" s="16">
+      <c r="J14" s="16">
         <v>15816813</v>
       </c>
-      <c r="F14" s="16">
+      <c r="K14" s="16">
         <v>20461979</v>
       </c>
-      <c r="G14" s="16">
+      <c r="L14" s="16">
         <v>59160218</v>
       </c>
-      <c r="H14" s="16">
-        <v>113204008</v>
+      <c r="M14" s="16">
+        <v>118261968</v>
       </c>
     </row>
     <row r="15">
@@ -566,18 +801,33 @@
         <v/>
       </c>
       <c r="D15" s="12">
+        <v>9643254</v>
+      </c>
+      <c r="E15" s="12">
+        <v>14542840</v>
+      </c>
+      <c r="F15" s="12">
+        <v>19531758</v>
+      </c>
+      <c r="G15" s="12">
+        <v>14677231</v>
+      </c>
+      <c r="H15" s="12">
+        <v>12991067</v>
+      </c>
+      <c r="I15" s="12">
         <v>12496977</v>
       </c>
-      <c r="E15" s="12">
+      <c r="J15" s="12">
         <v>31424662</v>
       </c>
-      <c r="F15" s="12">
+      <c r="K15" s="12">
         <v>53997362</v>
       </c>
-      <c r="G15" s="12">
+      <c r="L15" s="12">
         <v>79340060</v>
       </c>
-      <c r="H15" s="12">
+      <c r="M15" s="12">
         <v>134501506</v>
       </c>
     </row>
@@ -591,18 +841,33 @@
         <v/>
       </c>
       <c r="D16" s="16">
+        <v>3808198</v>
+      </c>
+      <c r="E16" s="16">
+        <v>2907976</v>
+      </c>
+      <c r="F16" s="16">
+        <v>1685181</v>
+      </c>
+      <c r="G16" s="16">
+        <v>843376</v>
+      </c>
+      <c r="H16" s="16">
+        <v>1348376</v>
+      </c>
+      <c r="I16" s="16">
         <v>2817886</v>
       </c>
-      <c r="E16" s="16">
+      <c r="J16" s="16">
         <v>13312826</v>
       </c>
-      <c r="F16" s="16">
+      <c r="K16" s="16">
         <v>2464327</v>
       </c>
-      <c r="G16" s="16">
+      <c r="L16" s="16">
         <v>3405080</v>
       </c>
-      <c r="H16" s="16">
+      <c r="M16" s="16">
         <v>9180700</v>
       </c>
     </row>
@@ -630,6 +895,21 @@
       <c r="H17" s="12">
         <v>0</v>
       </c>
+      <c r="I17" s="12">
+        <v>0</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <v>0</v>
+      </c>
+      <c r="M17" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" s="17" t="inlineStr">
@@ -641,19 +921,34 @@
         <v/>
       </c>
       <c r="D18" s="18">
+        <v>23770136</v>
+      </c>
+      <c r="E18" s="18">
+        <v>31211398</v>
+      </c>
+      <c r="F18" s="18">
+        <v>30859172</v>
+      </c>
+      <c r="G18" s="18">
+        <v>27273408</v>
+      </c>
+      <c r="H18" s="18">
+        <v>25868098</v>
+      </c>
+      <c r="I18" s="18">
         <v>30176969</v>
       </c>
-      <c r="E18" s="18">
+      <c r="J18" s="18">
         <v>66748245</v>
       </c>
-      <c r="F18" s="18">
+      <c r="K18" s="18">
         <v>87264387</v>
       </c>
-      <c r="G18" s="18">
+      <c r="L18" s="18">
         <v>176857509</v>
       </c>
-      <c r="H18" s="18">
-        <v>271091273</v>
+      <c r="M18" s="18">
+        <v>276149233</v>
       </c>
     </row>
     <row r="19">
@@ -666,18 +961,33 @@
         <v/>
       </c>
       <c r="D19" s="12">
+        <v>0</v>
+      </c>
+      <c r="E19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="12">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12">
+        <v>8099729</v>
+      </c>
+      <c r="H19" s="12">
+        <v>432962</v>
+      </c>
+      <c r="I19" s="12">
         <v>1735013</v>
       </c>
-      <c r="E19" s="12">
+      <c r="J19" s="12">
         <v>3647297</v>
       </c>
-      <c r="F19" s="12">
+      <c r="K19" s="12">
         <v>9503537</v>
       </c>
-      <c r="G19" s="12">
+      <c r="L19" s="12">
         <v>14303610</v>
       </c>
-      <c r="H19" s="12">
+      <c r="M19" s="12">
         <v>24830285</v>
       </c>
     </row>
@@ -691,18 +1001,33 @@
         <v/>
       </c>
       <c r="D20" s="16">
+        <v>526</v>
+      </c>
+      <c r="E20" s="16">
+        <v>4026</v>
+      </c>
+      <c r="F20" s="16">
+        <v>2373910</v>
+      </c>
+      <c r="G20" s="16">
+        <v>28714</v>
+      </c>
+      <c r="H20" s="16">
+        <v>5001221</v>
+      </c>
+      <c r="I20" s="16">
         <v>5028587</v>
       </c>
-      <c r="E20" s="16">
+      <c r="J20" s="16">
         <v>10051893</v>
       </c>
-      <c r="F20" s="16">
+      <c r="K20" s="16">
         <v>10275727</v>
       </c>
-      <c r="G20" s="16">
+      <c r="L20" s="16">
         <v>10285091</v>
       </c>
-      <c r="H20" s="16">
+      <c r="M20" s="16">
         <v>12659289</v>
       </c>
     </row>
@@ -715,11 +1040,15 @@
       <c r="C21" s="12">
         <v/>
       </c>
-      <c r="D21" s="12">
-        <v>0</v>
-      </c>
-      <c r="E21" s="12">
-        <v>0</v>
+      <c r="D21" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F21" s="12">
         <v>0</v>
@@ -728,6 +1057,21 @@
         <v>0</v>
       </c>
       <c r="H21" s="12">
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0</v>
+      </c>
+      <c r="K21" s="12">
+        <v>0</v>
+      </c>
+      <c r="L21" s="12">
+        <v>0</v>
+      </c>
+      <c r="M21" s="12">
         <v>0</v>
       </c>
     </row>
@@ -741,18 +1085,33 @@
         <v/>
       </c>
       <c r="D22" s="16">
+        <v>10914012</v>
+      </c>
+      <c r="E22" s="16">
+        <v>12747620</v>
+      </c>
+      <c r="F22" s="16">
+        <v>14692702</v>
+      </c>
+      <c r="G22" s="16">
+        <v>16650873</v>
+      </c>
+      <c r="H22" s="16">
+        <v>17991784</v>
+      </c>
+      <c r="I22" s="16">
         <v>19256032</v>
       </c>
-      <c r="E22" s="16">
+      <c r="J22" s="16">
         <v>21650916</v>
       </c>
-      <c r="F22" s="16">
+      <c r="K22" s="16">
         <v>27412453</v>
       </c>
-      <c r="G22" s="16">
+      <c r="L22" s="16">
         <v>47555160</v>
       </c>
-      <c r="H22" s="16">
+      <c r="M22" s="16">
         <v>85432406</v>
       </c>
     </row>
@@ -766,18 +1125,33 @@
         <v/>
       </c>
       <c r="D23" s="12">
+        <v>304465</v>
+      </c>
+      <c r="E23" s="12">
+        <v>305017</v>
+      </c>
+      <c r="F23" s="12">
+        <v>305407</v>
+      </c>
+      <c r="G23" s="12">
+        <v>305294</v>
+      </c>
+      <c r="H23" s="12">
+        <v>666552</v>
+      </c>
+      <c r="I23" s="12">
         <v>665738</v>
       </c>
-      <c r="E23" s="12">
+      <c r="J23" s="12">
         <v>683954</v>
       </c>
-      <c r="F23" s="12">
+      <c r="K23" s="12">
         <v>726494</v>
       </c>
-      <c r="G23" s="12">
+      <c r="L23" s="12">
         <v>725491</v>
       </c>
-      <c r="H23" s="12">
+      <c r="M23" s="12">
         <v>724811</v>
       </c>
     </row>
@@ -790,15 +1164,11 @@
       <c r="C24" s="16">
         <v/>
       </c>
-      <c r="D24" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E24" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D24" s="16">
+        <v>0</v>
+      </c>
+      <c r="E24" s="16">
+        <v>0</v>
       </c>
       <c r="F24" s="16" t="inlineStr">
         <is>
@@ -811,6 +1181,31 @@
         </is>
       </c>
       <c r="H24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L24" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M24" s="16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -826,18 +1221,33 @@
         <v/>
       </c>
       <c r="D25" s="12">
+        <v>61795</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1125787</v>
+      </c>
+      <c r="F25" s="12">
+        <v>7497843</v>
+      </c>
+      <c r="G25" s="12">
+        <v>2054655</v>
+      </c>
+      <c r="H25" s="12">
+        <v>2757414</v>
+      </c>
+      <c r="I25" s="12">
         <v>3354282</v>
       </c>
-      <c r="E25" s="12">
+      <c r="J25" s="12">
         <v>3048187</v>
       </c>
-      <c r="F25" s="12">
+      <c r="K25" s="12">
         <v>3351375</v>
       </c>
-      <c r="G25" s="12">
+      <c r="L25" s="12">
         <v>4228524</v>
       </c>
-      <c r="H25" s="12">
+      <c r="M25" s="12">
         <v>8971424</v>
       </c>
     </row>
@@ -851,18 +1261,33 @@
         <v/>
       </c>
       <c r="D26" s="18">
+        <v>11280798</v>
+      </c>
+      <c r="E26" s="18">
+        <v>14182450</v>
+      </c>
+      <c r="F26" s="18">
+        <v>24869862</v>
+      </c>
+      <c r="G26" s="18">
+        <v>27139265</v>
+      </c>
+      <c r="H26" s="18">
+        <v>26849933</v>
+      </c>
+      <c r="I26" s="18">
         <v>30039652</v>
       </c>
-      <c r="E26" s="18">
+      <c r="J26" s="18">
         <v>39082247</v>
       </c>
-      <c r="F26" s="18">
+      <c r="K26" s="18">
         <v>51269586</v>
       </c>
-      <c r="G26" s="18">
+      <c r="L26" s="18">
         <v>77097876</v>
       </c>
-      <c r="H26" s="18">
+      <c r="M26" s="18">
         <v>132618215</v>
       </c>
     </row>
@@ -876,19 +1301,34 @@
         <v/>
       </c>
       <c r="D27" s="20">
+        <v>35050934</v>
+      </c>
+      <c r="E27" s="20">
+        <v>45393848</v>
+      </c>
+      <c r="F27" s="20">
+        <v>55729034</v>
+      </c>
+      <c r="G27" s="20">
+        <v>54412673</v>
+      </c>
+      <c r="H27" s="20">
+        <v>52718031</v>
+      </c>
+      <c r="I27" s="20">
         <v>60216621</v>
       </c>
-      <c r="E27" s="20">
+      <c r="J27" s="20">
         <v>105830492</v>
       </c>
-      <c r="F27" s="20">
+      <c r="K27" s="20">
         <v>138533973</v>
       </c>
-      <c r="G27" s="20">
+      <c r="L27" s="20">
         <v>253955385</v>
       </c>
-      <c r="H27" s="20">
-        <v>403709488</v>
+      <c r="M27" s="20">
+        <v>408767448</v>
       </c>
     </row>
     <row r="28">
@@ -915,6 +1355,21 @@
       <c r="H28" s="14">
         <v/>
       </c>
+      <c r="I28" s="14">
+        <v/>
+      </c>
+      <c r="J28" s="14">
+        <v/>
+      </c>
+      <c r="K28" s="14">
+        <v/>
+      </c>
+      <c r="L28" s="14">
+        <v/>
+      </c>
+      <c r="M28" s="14">
+        <v/>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="15" t="inlineStr">
@@ -926,19 +1381,34 @@
         <v/>
       </c>
       <c r="D29" s="16">
+        <v>5199026</v>
+      </c>
+      <c r="E29" s="16">
+        <v>9662219</v>
+      </c>
+      <c r="F29" s="16">
+        <v>16564626</v>
+      </c>
+      <c r="G29" s="16">
+        <v>15544393</v>
+      </c>
+      <c r="H29" s="16">
+        <v>14710203</v>
+      </c>
+      <c r="I29" s="16">
         <v>13415055</v>
       </c>
-      <c r="E29" s="16">
+      <c r="J29" s="16">
         <v>30937615</v>
       </c>
-      <c r="F29" s="16">
+      <c r="K29" s="16">
         <v>39174462</v>
       </c>
-      <c r="G29" s="16">
+      <c r="L29" s="16">
         <v>40466304</v>
       </c>
-      <c r="H29" s="16">
-        <v>100303238</v>
+      <c r="M29" s="16">
+        <v>105361198</v>
       </c>
     </row>
     <row r="30">
@@ -950,15 +1420,11 @@
       <c r="C30" s="12">
         <v/>
       </c>
-      <c r="D30" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E30" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="D30" s="12">
+        <v>0</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0</v>
       </c>
       <c r="F30" s="12" t="inlineStr">
         <is>
@@ -971,6 +1437,31 @@
         </is>
       </c>
       <c r="H30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L30" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M30" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -986,18 +1477,33 @@
         <v/>
       </c>
       <c r="D31" s="16">
+        <v>1969318</v>
+      </c>
+      <c r="E31" s="16">
+        <v>676162</v>
+      </c>
+      <c r="F31" s="16">
+        <v>156572</v>
+      </c>
+      <c r="G31" s="16">
+        <v>328152</v>
+      </c>
+      <c r="H31" s="16">
+        <v>1746891</v>
+      </c>
+      <c r="I31" s="16">
         <v>2014189</v>
       </c>
-      <c r="E31" s="16">
+      <c r="J31" s="16">
         <v>4340785</v>
       </c>
-      <c r="F31" s="16">
+      <c r="K31" s="16">
         <v>14836419</v>
       </c>
-      <c r="G31" s="16">
+      <c r="L31" s="16">
         <v>19541138</v>
       </c>
-      <c r="H31" s="16">
+      <c r="M31" s="16">
         <v>19290144</v>
       </c>
     </row>
@@ -1011,18 +1517,33 @@
         <v/>
       </c>
       <c r="D32" s="12">
+        <v>3446072</v>
+      </c>
+      <c r="E32" s="12">
+        <v>4475568</v>
+      </c>
+      <c r="F32" s="12">
+        <v>3101534</v>
+      </c>
+      <c r="G32" s="12">
+        <v>2229990</v>
+      </c>
+      <c r="H32" s="12">
+        <v>1422967</v>
+      </c>
+      <c r="I32" s="12">
         <v>1055212</v>
       </c>
-      <c r="E32" s="12">
+      <c r="J32" s="12">
         <v>1695129</v>
       </c>
-      <c r="F32" s="12">
+      <c r="K32" s="12">
         <v>2595793</v>
       </c>
-      <c r="G32" s="12">
+      <c r="L32" s="12">
         <v>3988256</v>
       </c>
-      <c r="H32" s="12">
+      <c r="M32" s="12">
         <v>9145967</v>
       </c>
     </row>
@@ -1036,18 +1557,33 @@
         <v/>
       </c>
       <c r="D33" s="16">
+        <v>1533877</v>
+      </c>
+      <c r="E33" s="16">
+        <v>1193818</v>
+      </c>
+      <c r="F33" s="16">
+        <v>6565844</v>
+      </c>
+      <c r="G33" s="16">
+        <v>13891881</v>
+      </c>
+      <c r="H33" s="16">
+        <v>2236922</v>
+      </c>
+      <c r="I33" s="16">
         <v>1090990</v>
       </c>
-      <c r="E33" s="16">
+      <c r="J33" s="16">
         <v>3019277</v>
       </c>
-      <c r="F33" s="16">
+      <c r="K33" s="16">
         <v>2197494</v>
       </c>
-      <c r="G33" s="16">
+      <c r="L33" s="16">
         <v>269729</v>
       </c>
-      <c r="H33" s="16">
+      <c r="M33" s="16">
         <v>2731447</v>
       </c>
     </row>
@@ -1061,18 +1597,33 @@
         <v/>
       </c>
       <c r="D34" s="12">
+        <v>1316026</v>
+      </c>
+      <c r="E34" s="12">
+        <v>3075474</v>
+      </c>
+      <c r="F34" s="12">
+        <v>7100663</v>
+      </c>
+      <c r="G34" s="12">
+        <v>7455134</v>
+      </c>
+      <c r="H34" s="12">
+        <v>8004371</v>
+      </c>
+      <c r="I34" s="12">
         <v>8036752</v>
       </c>
-      <c r="E34" s="12">
+      <c r="J34" s="12">
         <v>10391784</v>
       </c>
-      <c r="F34" s="12">
+      <c r="K34" s="12">
         <v>8881662</v>
       </c>
-      <c r="G34" s="12">
+      <c r="L34" s="12">
         <v>8297115</v>
       </c>
-      <c r="H34" s="12">
+      <c r="M34" s="12">
         <v>5314548</v>
       </c>
     </row>
@@ -1085,11 +1636,15 @@
       <c r="C35" s="16">
         <v/>
       </c>
-      <c r="D35" s="16">
-        <v>0</v>
-      </c>
-      <c r="E35" s="16">
-        <v>0</v>
+      <c r="D35" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F35" s="16">
         <v>0</v>
@@ -1098,6 +1653,21 @@
         <v>0</v>
       </c>
       <c r="H35" s="16">
+        <v>0</v>
+      </c>
+      <c r="I35" s="16">
+        <v>0</v>
+      </c>
+      <c r="J35" s="16">
+        <v>0</v>
+      </c>
+      <c r="K35" s="16">
+        <v>0</v>
+      </c>
+      <c r="L35" s="16">
+        <v>0</v>
+      </c>
+      <c r="M35" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1125,6 +1695,21 @@
       <c r="H36" s="12">
         <v>0</v>
       </c>
+      <c r="I36" s="12">
+        <v>0</v>
+      </c>
+      <c r="J36" s="12">
+        <v>0</v>
+      </c>
+      <c r="K36" s="12">
+        <v>0</v>
+      </c>
+      <c r="L36" s="12">
+        <v>0</v>
+      </c>
+      <c r="M36" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="17" t="inlineStr">
@@ -1136,19 +1721,34 @@
         <v/>
       </c>
       <c r="D37" s="18">
+        <v>13464319</v>
+      </c>
+      <c r="E37" s="18">
+        <v>19083241</v>
+      </c>
+      <c r="F37" s="18">
+        <v>33489239</v>
+      </c>
+      <c r="G37" s="18">
+        <v>39449550</v>
+      </c>
+      <c r="H37" s="18">
+        <v>28121354</v>
+      </c>
+      <c r="I37" s="18">
         <v>25612198</v>
       </c>
-      <c r="E37" s="18">
+      <c r="J37" s="18">
         <v>50384590</v>
       </c>
-      <c r="F37" s="18">
+      <c r="K37" s="18">
         <v>67685830</v>
       </c>
-      <c r="G37" s="18">
+      <c r="L37" s="18">
         <v>72562542</v>
       </c>
-      <c r="H37" s="18">
-        <v>136785344</v>
+      <c r="M37" s="18">
+        <v>141843304</v>
       </c>
     </row>
     <row r="38">
@@ -1161,18 +1761,33 @@
         <v/>
       </c>
       <c r="D38" s="12">
+        <v>0</v>
+      </c>
+      <c r="E38" s="12">
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <v>9084</v>
+      </c>
+      <c r="G38" s="12">
+        <v>5400</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12">
         <v>18522</v>
       </c>
-      <c r="E38" s="12">
-        <v>0</v>
-      </c>
-      <c r="F38" s="12">
-        <v>0</v>
-      </c>
-      <c r="G38" s="12">
+      <c r="J38" s="12">
+        <v>0</v>
+      </c>
+      <c r="K38" s="12">
+        <v>0</v>
+      </c>
+      <c r="L38" s="12">
         <v>7504712</v>
       </c>
-      <c r="H38" s="12">
+      <c r="M38" s="12">
         <v>9185745</v>
       </c>
     </row>
@@ -1185,25 +1800,44 @@
       <c r="C39" s="16">
         <v/>
       </c>
-      <c r="D39" s="16">
-        <v>0</v>
+      <c r="D39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="E39" s="16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F39" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G39" s="16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H39" s="16" t="inlineStr">
+      <c r="F39" s="16">
+        <v>0</v>
+      </c>
+      <c r="G39" s="16">
+        <v>0</v>
+      </c>
+      <c r="H39" s="16">
+        <v>0</v>
+      </c>
+      <c r="I39" s="16">
+        <v>0</v>
+      </c>
+      <c r="J39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L39" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M39" s="16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1219,18 +1853,33 @@
         <v/>
       </c>
       <c r="D40" s="12">
-        <v>0</v>
+        <v>794847</v>
       </c>
       <c r="E40" s="12">
-        <v>0</v>
+        <v>257259</v>
       </c>
       <c r="F40" s="12">
-        <v>0</v>
+        <v>53821</v>
       </c>
       <c r="G40" s="12">
-        <v>0</v>
+        <v>30547</v>
       </c>
       <c r="H40" s="12">
+        <v>0</v>
+      </c>
+      <c r="I40" s="12">
+        <v>0</v>
+      </c>
+      <c r="J40" s="12">
+        <v>0</v>
+      </c>
+      <c r="K40" s="12">
+        <v>0</v>
+      </c>
+      <c r="L40" s="12">
+        <v>0</v>
+      </c>
+      <c r="M40" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1244,18 +1893,33 @@
         <v/>
       </c>
       <c r="D41" s="16">
+        <v>840384</v>
+      </c>
+      <c r="E41" s="16">
+        <v>1128861</v>
+      </c>
+      <c r="F41" s="16">
+        <v>1384898</v>
+      </c>
+      <c r="G41" s="16">
+        <v>1615105</v>
+      </c>
+      <c r="H41" s="16">
+        <v>1548935</v>
+      </c>
+      <c r="I41" s="16">
         <v>1543157</v>
       </c>
-      <c r="E41" s="16">
+      <c r="J41" s="16">
         <v>1706789</v>
       </c>
-      <c r="F41" s="16">
+      <c r="K41" s="16">
         <v>2761856</v>
       </c>
-      <c r="G41" s="16">
+      <c r="L41" s="16">
         <v>4239971</v>
       </c>
-      <c r="H41" s="16">
+      <c r="M41" s="16">
         <v>7075705</v>
       </c>
     </row>
@@ -1269,18 +1933,33 @@
         <v/>
       </c>
       <c r="D42" s="20">
+        <v>1635231</v>
+      </c>
+      <c r="E42" s="20">
+        <v>1386120</v>
+      </c>
+      <c r="F42" s="20">
+        <v>1447803</v>
+      </c>
+      <c r="G42" s="20">
+        <v>1651052</v>
+      </c>
+      <c r="H42" s="20">
+        <v>1548935</v>
+      </c>
+      <c r="I42" s="20">
         <v>1561679</v>
       </c>
-      <c r="E42" s="20">
+      <c r="J42" s="20">
         <v>1706789</v>
       </c>
-      <c r="F42" s="20">
+      <c r="K42" s="20">
         <v>2761856</v>
       </c>
-      <c r="G42" s="20">
+      <c r="L42" s="20">
         <v>11744683</v>
       </c>
-      <c r="H42" s="20">
+      <c r="M42" s="20">
         <v>16261450</v>
       </c>
     </row>
@@ -1294,19 +1973,34 @@
         <v/>
       </c>
       <c r="D43" s="18">
+        <v>15099550</v>
+      </c>
+      <c r="E43" s="18">
+        <v>20469361</v>
+      </c>
+      <c r="F43" s="18">
+        <v>34937042</v>
+      </c>
+      <c r="G43" s="18">
+        <v>41100602</v>
+      </c>
+      <c r="H43" s="18">
+        <v>29670289</v>
+      </c>
+      <c r="I43" s="18">
         <v>27173877</v>
       </c>
-      <c r="E43" s="18">
+      <c r="J43" s="18">
         <v>52091379</v>
       </c>
-      <c r="F43" s="18">
+      <c r="K43" s="18">
         <v>70447686</v>
       </c>
-      <c r="G43" s="18">
+      <c r="L43" s="18">
         <v>84307225</v>
       </c>
-      <c r="H43" s="18">
-        <v>153046794</v>
+      <c r="M43" s="18">
+        <v>158104754</v>
       </c>
     </row>
     <row r="44">
@@ -1333,6 +2027,21 @@
       <c r="H44" s="14">
         <v/>
       </c>
+      <c r="I44" s="14">
+        <v/>
+      </c>
+      <c r="J44" s="14">
+        <v/>
+      </c>
+      <c r="K44" s="14">
+        <v/>
+      </c>
+      <c r="L44" s="14">
+        <v/>
+      </c>
+      <c r="M44" s="14">
+        <v/>
+      </c>
     </row>
     <row r="45">
       <c r="B45" s="15" t="inlineStr">
@@ -1344,18 +2053,33 @@
         <v/>
       </c>
       <c r="D45" s="16">
+        <v>2192000</v>
+      </c>
+      <c r="E45" s="16">
+        <v>8000000</v>
+      </c>
+      <c r="F45" s="16">
+        <v>8000000</v>
+      </c>
+      <c r="G45" s="16">
+        <v>8000000</v>
+      </c>
+      <c r="H45" s="16">
         <v>14472000</v>
       </c>
-      <c r="E45" s="16">
+      <c r="I45" s="16">
+        <v>14472000</v>
+      </c>
+      <c r="J45" s="16">
         <v>19048697</v>
       </c>
-      <c r="F45" s="16">
+      <c r="K45" s="16">
         <v>19048697</v>
       </c>
-      <c r="G45" s="16">
+      <c r="L45" s="16">
         <v>50000000</v>
       </c>
-      <c r="H45" s="16">
+      <c r="M45" s="16">
         <v>120000000</v>
       </c>
     </row>
@@ -1383,6 +2107,21 @@
       <c r="H46" s="12">
         <v>0</v>
       </c>
+      <c r="I46" s="12">
+        <v>0</v>
+      </c>
+      <c r="J46" s="12">
+        <v>0</v>
+      </c>
+      <c r="K46" s="12">
+        <v>0</v>
+      </c>
+      <c r="L46" s="12">
+        <v>0</v>
+      </c>
+      <c r="M46" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="15" t="inlineStr">
@@ -1403,9 +2142,24 @@
         <v>0</v>
       </c>
       <c r="G47" s="16">
-        <v>0</v>
+        <v>352011</v>
       </c>
       <c r="H47" s="16">
+        <v>0</v>
+      </c>
+      <c r="I47" s="16">
+        <v>0</v>
+      </c>
+      <c r="J47" s="16">
+        <v>0</v>
+      </c>
+      <c r="K47" s="16">
+        <v>0</v>
+      </c>
+      <c r="L47" s="16">
+        <v>0</v>
+      </c>
+      <c r="M47" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1418,11 +2172,15 @@
       <c r="C48" s="12">
         <v/>
       </c>
-      <c r="D48" s="12">
-        <v>0</v>
-      </c>
-      <c r="E48" s="12">
-        <v>0</v>
+      <c r="D48" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E48" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F48" s="12">
         <v>0</v>
@@ -1431,6 +2189,21 @@
         <v>0</v>
       </c>
       <c r="H48" s="12">
+        <v>0</v>
+      </c>
+      <c r="I48" s="12">
+        <v>0</v>
+      </c>
+      <c r="J48" s="12">
+        <v>0</v>
+      </c>
+      <c r="K48" s="12">
+        <v>0</v>
+      </c>
+      <c r="L48" s="12">
+        <v>0</v>
+      </c>
+      <c r="M48" s="12">
         <v>-4437327</v>
       </c>
     </row>
@@ -1448,16 +2221,41 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E49" s="16">
-        <v>0</v>
-      </c>
-      <c r="F49" s="16">
-        <v>0</v>
-      </c>
-      <c r="G49" s="16">
-        <v>0</v>
-      </c>
-      <c r="H49" s="16">
+      <c r="E49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I49" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J49" s="16">
+        <v>0</v>
+      </c>
+      <c r="K49" s="16">
+        <v>0</v>
+      </c>
+      <c r="L49" s="16">
+        <v>0</v>
+      </c>
+      <c r="M49" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1471,18 +2269,33 @@
         <v/>
       </c>
       <c r="D50" s="12">
+        <v>384695</v>
+      </c>
+      <c r="E50" s="12">
+        <v>800000</v>
+      </c>
+      <c r="F50" s="12">
+        <v>800000</v>
+      </c>
+      <c r="G50" s="12">
+        <v>800000</v>
+      </c>
+      <c r="H50" s="12">
+        <v>1123356</v>
+      </c>
+      <c r="I50" s="12">
         <v>1447200</v>
       </c>
-      <c r="E50" s="12">
+      <c r="J50" s="12">
         <v>1904870</v>
       </c>
-      <c r="F50" s="12">
+      <c r="K50" s="12">
         <v>1904870</v>
       </c>
-      <c r="G50" s="12">
+      <c r="L50" s="12">
         <v>5000000</v>
       </c>
-      <c r="H50" s="12">
+      <c r="M50" s="12">
         <v>12000000</v>
       </c>
     </row>
@@ -1496,7 +2309,7 @@
         <v/>
       </c>
       <c r="D51" s="16">
-        <v>43798</v>
+        <v>171616</v>
       </c>
       <c r="E51" s="16">
         <v>43798</v>
@@ -1510,6 +2323,21 @@
       <c r="H51" s="16">
         <v>43798</v>
       </c>
+      <c r="I51" s="16">
+        <v>43798</v>
+      </c>
+      <c r="J51" s="16">
+        <v>43798</v>
+      </c>
+      <c r="K51" s="16">
+        <v>43798</v>
+      </c>
+      <c r="L51" s="16">
+        <v>43798</v>
+      </c>
+      <c r="M51" s="16">
+        <v>43798</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" s="11" t="inlineStr">
@@ -1523,22 +2351,37 @@
       <c r="D52" s="12">
         <v>0</v>
       </c>
-      <c r="E52" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F52" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G52" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H52" s="12" t="inlineStr">
+      <c r="E52" s="12">
+        <v>0</v>
+      </c>
+      <c r="F52" s="12">
+        <v>0</v>
+      </c>
+      <c r="G52" s="12">
+        <v>0</v>
+      </c>
+      <c r="H52" s="12">
+        <v>0</v>
+      </c>
+      <c r="I52" s="12">
+        <v>0</v>
+      </c>
+      <c r="J52" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K52" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L52" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M52" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1568,6 +2411,21 @@
       <c r="H53" s="16">
         <v>0</v>
       </c>
+      <c r="I53" s="16">
+        <v>0</v>
+      </c>
+      <c r="J53" s="16">
+        <v>0</v>
+      </c>
+      <c r="K53" s="16">
+        <v>0</v>
+      </c>
+      <c r="L53" s="16">
+        <v>0</v>
+      </c>
+      <c r="M53" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="B54" s="11" t="inlineStr">
@@ -1581,22 +2439,37 @@
       <c r="D54" s="12">
         <v>0</v>
       </c>
-      <c r="E54" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F54" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G54" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H54" s="12" t="inlineStr">
+      <c r="E54" s="12">
+        <v>0</v>
+      </c>
+      <c r="F54" s="12">
+        <v>0</v>
+      </c>
+      <c r="G54" s="12">
+        <v>0</v>
+      </c>
+      <c r="H54" s="12">
+        <v>0</v>
+      </c>
+      <c r="I54" s="12">
+        <v>0</v>
+      </c>
+      <c r="J54" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K54" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L54" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M54" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1611,11 +2484,15 @@
       <c r="C55" s="16">
         <v/>
       </c>
-      <c r="D55" s="16">
-        <v>0</v>
-      </c>
-      <c r="E55" s="16">
-        <v>0</v>
+      <c r="D55" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E55" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="F55" s="16">
         <v>0</v>
@@ -1624,6 +2501,21 @@
         <v>0</v>
       </c>
       <c r="H55" s="16">
+        <v>0</v>
+      </c>
+      <c r="I55" s="16">
+        <v>0</v>
+      </c>
+      <c r="J55" s="16">
+        <v>0</v>
+      </c>
+      <c r="K55" s="16">
+        <v>0</v>
+      </c>
+      <c r="L55" s="16">
+        <v>0</v>
+      </c>
+      <c r="M55" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1637,18 +2529,33 @@
         <v/>
       </c>
       <c r="D56" s="12">
+        <v>17203073</v>
+      </c>
+      <c r="E56" s="12">
+        <v>16080689</v>
+      </c>
+      <c r="F56" s="12">
+        <v>11948194</v>
+      </c>
+      <c r="G56" s="12">
+        <v>4116262</v>
+      </c>
+      <c r="H56" s="12">
+        <v>7408588</v>
+      </c>
+      <c r="I56" s="12">
         <v>17079746</v>
       </c>
-      <c r="E56" s="12">
+      <c r="J56" s="12">
         <v>32741748</v>
       </c>
-      <c r="F56" s="12">
+      <c r="K56" s="12">
         <v>47088922</v>
       </c>
-      <c r="G56" s="12">
+      <c r="L56" s="12">
         <v>114604362</v>
       </c>
-      <c r="H56" s="12">
+      <c r="M56" s="12">
         <v>123056223</v>
       </c>
     </row>
@@ -1662,18 +2569,33 @@
         <v/>
       </c>
       <c r="D57" s="18">
+        <v>19951384</v>
+      </c>
+      <c r="E57" s="18">
+        <v>24924487</v>
+      </c>
+      <c r="F57" s="18">
+        <v>20791992</v>
+      </c>
+      <c r="G57" s="18">
+        <v>13312071</v>
+      </c>
+      <c r="H57" s="18">
+        <v>23047742</v>
+      </c>
+      <c r="I57" s="18">
         <v>33042744</v>
       </c>
-      <c r="E57" s="18">
+      <c r="J57" s="18">
         <v>53739113</v>
       </c>
-      <c r="F57" s="18">
+      <c r="K57" s="18">
         <v>68086287</v>
       </c>
-      <c r="G57" s="18">
+      <c r="L57" s="18">
         <v>169648160</v>
       </c>
-      <c r="H57" s="18">
+      <c r="M57" s="18">
         <v>250662694</v>
       </c>
     </row>
@@ -1687,19 +2609,34 @@
         <v/>
       </c>
       <c r="D58" s="20">
+        <v>35050934</v>
+      </c>
+      <c r="E58" s="20">
+        <v>45393848</v>
+      </c>
+      <c r="F58" s="20">
+        <v>55729034</v>
+      </c>
+      <c r="G58" s="20">
+        <v>54412673</v>
+      </c>
+      <c r="H58" s="20">
+        <v>52718031</v>
+      </c>
+      <c r="I58" s="20">
         <v>60216621</v>
       </c>
-      <c r="E58" s="20">
+      <c r="J58" s="20">
         <v>105830492</v>
       </c>
-      <c r="F58" s="20">
+      <c r="K58" s="20">
         <v>138533973</v>
       </c>
-      <c r="G58" s="20">
+      <c r="L58" s="20">
         <v>253955385</v>
       </c>
-      <c r="H58" s="20">
-        <v>403709488</v>
+      <c r="M58" s="20">
+        <v>408767448</v>
       </c>
     </row>
     <row r="59">
@@ -1722,6 +2659,21 @@
         <v/>
       </c>
       <c r="H59" s="2">
+        <v/>
+      </c>
+      <c r="I59" s="2">
+        <v/>
+      </c>
+      <c r="J59" s="2">
+        <v/>
+      </c>
+      <c r="K59" s="2">
+        <v/>
+      </c>
+      <c r="L59" s="2">
+        <v/>
+      </c>
+      <c r="M59" s="2">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
add auto arima to code
</commit_message>
<xml_diff>
--- a/database/industries/folad/fakhouz/balancesheet/yearly.xlsx
+++ b/database/industries/folad/fakhouz/balancesheet/yearly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\VAHID\Desktop\Trade\database\industries\folad\fakhouz\balancesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C966EB4-3AAA-4103-8ACF-C01A70D9D2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B423E451-007A-4735-8E6B-DDCF32964BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="708" yWindow="708" windowWidth="18204" windowHeight="11532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="18204" windowHeight="11532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>

</xml_diff>